<commit_message>
summarize # of samples in cbc samples
</commit_message>
<xml_diff>
--- a/2019_2022_resequencing/ThijsNB.xlsx
+++ b/2019_2022_resequencing/ThijsNB.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookesienkiewicz/Documents/sctld/metagenomic_analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brookesienkiewicz/Documents/LabNotebook/2019_2022_resequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F286CD58-324C-0343-B13C-A898D24E4E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A98C266-6C04-9F4C-80E0-9122C787B4E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{C50714DA-DC49-D241-9A22-E995A91432E7}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C50714DA-DC49-D241-9A22-E995A91432E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -220,7 +220,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -237,12 +237,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -266,17 +272,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D365CD-8C39-5D40-B2FA-043C0875B406}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <selection activeCell="A13" activeCellId="1" sqref="A8:XFD8 A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,54 +994,55 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
+    <row r="8" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="str">
         <f t="shared" si="0"/>
         <v>62019_T3_1_MCAV</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="10">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="10">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="11">
         <v>43617</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="12">
         <v>62019</v>
       </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8">
+      <c r="H8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="10">
         <v>113</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="13">
         <v>44725</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="10">
         <v>3.9</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="13">
         <v>44743</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="10">
         <v>0.6</v>
       </c>
-      <c r="Q8" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="O8" s="14"/>
+      <c r="Q8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1229,57 +1241,57 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
+    <row r="13" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="str">
         <f t="shared" si="0"/>
         <v>052022_T3_1_MCAV</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="10">
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <v>1</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="11">
         <v>44682</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="H13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="13">
         <v>44727</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="10">
         <v>37</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="13">
         <v>44734</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="10">
         <v>3.6</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="14">
         <v>1.8</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="13">
         <v>44739</v>
       </c>
-      <c r="Q13" t="s">
-        <v>16</v>
-      </c>
-      <c r="R13" t="s">
+      <c r="Q13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R13" s="10" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>